<commit_message>
Made changes to the two columns and changed some codes.
I decided to pick two other variables for the example2 dataset. The ones I had picked previously didn't make much sense for the dataset. I also edited some of the codes from part 2 of the assignment.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE57AFD0-5AB7-B341-A5DD-7949FD600E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CFDFFE-D832-164B-A750-30566A880A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Height</t>
   </si>
@@ -74,31 +74,37 @@
     <t>identified gender (male/female/other)</t>
   </si>
   <si>
-    <t>Race</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>BMI</t>
-  </si>
-  <si>
-    <t>identified race (Black, White, Asian, Latino)</t>
-  </si>
-  <si>
-    <t>B/W/A/L</t>
-  </si>
-  <si>
-    <t>body mass index ranging from 15 to 34</t>
+    <t>Resting Heart Rate</t>
+  </si>
+  <si>
+    <t>Heart rate when resting ranging from 40 to 153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric value &gt;0 </t>
+  </si>
+  <si>
+    <t>Cardio</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Yoga</t>
+  </si>
+  <si>
+    <t>Strength training</t>
+  </si>
+  <si>
+    <t>Cardio/Strength training /Yoga/None</t>
+  </si>
+  <si>
+    <t>Preferred exercise Type</t>
+  </si>
+  <si>
+    <t>Preferred exercise type (Cardio, Strenght training, Yoga, None)</t>
+  </si>
+  <si>
+    <t>Preferred exercise type</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,14 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -447,10 +457,10 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -464,10 +474,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -481,10 +491,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -498,10 +508,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2">
-        <v>34</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -515,10 +525,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2">
-        <v>21</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -532,10 +542,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
-        <v>23</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -549,10 +559,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -566,10 +576,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2">
-        <v>21</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -586,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="2">
-        <v>24</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -603,7 +613,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="2">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -617,10 +627,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2">
-        <v>23</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -631,10 +641,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -648,10 +658,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -665,10 +675,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2">
-        <v>31</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -682,10 +692,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E15" s="2">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -697,15 +707,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="277" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="173" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -754,10 +764,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -765,13 +775,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>